<commit_message>
Finish UartProtocol.cs and test in bench
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -82,27 +82,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Actual (beyond plan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>%</t>
     </r>
     <r>
@@ -238,6 +217,28 @@
   </si>
   <si>
     <t>Test in eqiupemnt</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Actual (beyond plan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1063,8 +1064,8 @@
   </sheetPr>
   <dimension ref="B1:BN16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1089,27 +1090,27 @@
     </row>
     <row r="2" spans="2:66" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" s="26">
-        <v>42797</v>
+        <v>42798</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="21"/>
       <c r="M2" s="20"/>
       <c r="N2" s="13"/>
       <c r="O2" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -1121,14 +1122,14 @@
       <c r="U2" s="23"/>
       <c r="V2" s="15"/>
       <c r="W2" s="22" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
       <c r="Z2" s="23"/>
       <c r="AA2" s="16"/>
       <c r="AB2" s="29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="30"/>
       <c r="AD2" s="30"/>
@@ -1143,22 +1144,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="E3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="G3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>10</v>
-      </c>
       <c r="H3" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="8"/>
@@ -1367,7 +1368,7 @@
     </row>
     <row r="5" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="27">
         <v>42797</v>
@@ -1379,16 +1380,16 @@
         <v>42797</v>
       </c>
       <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6">
         <v>1</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.4</v>
       </c>
       <c r="AA5"/>
     </row>
     <row r="6" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="27">
         <v>42800</v>
@@ -1399,13 +1400,13 @@
       <c r="E6" s="27"/>
       <c r="F6" s="5"/>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6"/>
     </row>
     <row r="7" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="27">
         <v>42806</v>
@@ -1413,16 +1414,20 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="27">
+        <v>42798</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="G7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7"/>
     </row>
     <row r="8" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="27">
         <v>42806</v>
@@ -1443,7 +1448,7 @@
     </row>
     <row r="9" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="27">
         <v>42806</v>
@@ -1460,7 +1465,7 @@
     </row>
     <row r="10" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="27">
         <v>42809</v>
@@ -1477,7 +1482,7 @@
     </row>
     <row r="11" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="27">
         <v>42812</v>
@@ -1494,7 +1499,7 @@
     </row>
     <row r="12" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="27">
         <v>42813</v>
@@ -1511,7 +1516,7 @@
     </row>
     <row r="13" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="27">
         <v>42813</v>
@@ -1528,7 +1533,7 @@
     </row>
     <row r="14" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="27">
         <v>42814</v>
@@ -1545,7 +1550,7 @@
     </row>
     <row r="15" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="27">
         <v>42815</v>
@@ -1562,7 +1567,7 @@
     </row>
     <row r="16" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="27">
         <v>42819</v>

</xml_diff>

<commit_message>
Add plan and folder for Labview reconstruction.
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="4710" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Project Planner</t>
   </si>
@@ -239,6 +239,10 @@
       </rPr>
       <t>)</t>
     </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Labview reconstruction</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1062,16 +1066,16 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BN16"/>
+  <dimension ref="B1:BN17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="3" customWidth="1"/>
     <col min="8" max="27" width="4.625" style="1" customWidth="1"/>
@@ -1582,6 +1586,23 @@
       </c>
       <c r="AA16"/>
     </row>
+    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="27">
+        <v>42821</v>
+      </c>
+      <c r="D17" s="5">
+        <v>15</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA17"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="AB2:AI2"/>
@@ -1594,7 +1615,7 @@
     <mergeCell ref="G3:G4"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="H5:BN16">
+  <conditionalFormatting sqref="H5:BN17">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1620,7 +1641,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:BO17">
+  <conditionalFormatting sqref="B18:BO18">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finish 40% ParameterSet form & create GlobalVars.uartCom & Add tempThr into parameter list
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="8430" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1078,7 +1078,7 @@
   <dimension ref="B1:BN17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="26">
-        <v>42805</v>
+        <v>42806</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="19" t="s">
@@ -1528,10 +1528,14 @@
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="27">
+        <v>42806</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AA12"/>
     </row>

</xml_diff>

<commit_message>
Add parameter update implement and save data to file class
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8430" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Roy</author>
+  </authors>
+  <commentList>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Roy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Waste too much time not working</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Project Planner</t>
   </si>
@@ -136,38 +172,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ART protocol</t>
-    </r>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>tep Control</t>
-    </r>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>Test bench</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -177,22 +181,6 @@
   </si>
   <si>
     <t>Auto Form</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>anual Form</t>
-    </r>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
@@ -242,7 +230,31 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Labview reconstruction</t>
+    <t>c#</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>托管和非托管，资源释放</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>control</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>chart</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>UART protocol</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step Control</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual Form</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -361,8 +373,46 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +464,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -494,7 +549,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,8 +605,11 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,8 +724,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="% complete" xfId="16"/>
     <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
     <cellStyle name="Activity" xfId="2"/>
@@ -686,6 +750,7 @@
     <cellStyle name="标题 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
     <cellStyle name="解释性文本" xfId="12" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
@@ -1070,15 +1135,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BN17"/>
+  <dimension ref="B1:BN16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1200,7 @@
       <c r="U2" s="23"/>
       <c r="V2" s="15"/>
       <c r="W2" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
@@ -1380,8 +1445,8 @@
       </c>
     </row>
     <row r="5" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
-        <v>14</v>
+      <c r="B5" s="39" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="27">
         <v>42797</v>
@@ -1401,8 +1466,8 @@
       <c r="AA5"/>
     </row>
     <row r="6" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
-        <v>15</v>
+      <c r="B6" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C6" s="27">
         <v>42800</v>
@@ -1422,11 +1487,11 @@
       <c r="AA6"/>
     </row>
     <row r="7" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
-        <v>16</v>
+      <c r="B7" s="39" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="27">
-        <v>42806</v>
+        <v>42807</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -1443,11 +1508,11 @@
       <c r="AA7"/>
     </row>
     <row r="8" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
-        <v>17</v>
+      <c r="B8" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="27">
-        <v>42806</v>
+        <v>42807</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -1464,93 +1529,105 @@
       <c r="AA8"/>
     </row>
     <row r="9" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18" t="s">
-        <v>18</v>
+      <c r="B9" s="39" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="27">
-        <v>42806</v>
+        <v>42805</v>
       </c>
       <c r="D9" s="5">
-        <v>3</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="27">
+        <v>42805</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9"/>
     </row>
     <row r="10" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="27">
-        <v>42809</v>
+        <v>42806</v>
       </c>
       <c r="D10" s="5">
-        <v>4</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="27">
+        <v>42806</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
       <c r="G10" s="6">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AA10"/>
     </row>
     <row r="11" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="27">
-        <v>42812</v>
+        <v>42806</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
       </c>
       <c r="E11" s="27">
-        <v>42805</v>
+        <v>42807</v>
       </c>
       <c r="F11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA11"/>
     </row>
     <row r="12" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" s="27">
-        <v>42813</v>
+        <v>42807</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" s="27">
-        <v>42806</v>
+        <v>42809</v>
       </c>
       <c r="F12" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AA12"/>
     </row>
     <row r="13" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C13" s="27">
+        <v>42810</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
+      </c>
+      <c r="E13" s="27">
         <v>42813</v>
       </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>3</v>
+      </c>
       <c r="G13" s="6">
         <v>0</v>
       </c>
@@ -1558,7 +1635,7 @@
     </row>
     <row r="14" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="27">
         <v>42814</v>
@@ -1566,8 +1643,12 @@
       <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="27">
+        <v>42816</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2</v>
+      </c>
       <c r="G14" s="6">
         <v>0</v>
       </c>
@@ -1575,7 +1656,7 @@
     </row>
     <row r="15" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="27">
         <v>42815</v>
@@ -1583,8 +1664,12 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="27">
+        <v>42818</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -1592,7 +1677,7 @@
     </row>
     <row r="16" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="27">
         <v>42819</v>
@@ -1600,29 +1685,16 @@
       <c r="D16" s="5">
         <v>2</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="27">
+        <v>42819</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
       <c r="G16" s="6">
         <v>0</v>
       </c>
       <c r="AA16"/>
-    </row>
-    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="27">
-        <v>42821</v>
-      </c>
-      <c r="D17" s="5">
-        <v>15</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1636,7 +1708,7 @@
     <mergeCell ref="G3:G4"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="H5:BN17">
+  <conditionalFormatting sqref="H5:BN16">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1662,7 +1734,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:BO18">
+  <conditionalFormatting sqref="B17:BO17">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -1698,6 +1770,7 @@
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1711,15 +1784,36 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish ParameterSet and LogShow
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="10290" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Project Planner</t>
   </si>
@@ -188,14 +188,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Para Form</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Log Form</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>Config.ini</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -255,6 +247,22 @@
   </si>
   <si>
     <t>Manual Form</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Para Form</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log Form</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>c#</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>delegate and invoke</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -700,6 +708,12 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -723,12 +737,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1143,7 +1151,7 @@
   <dimension ref="B1:BN16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1167,13 +1175,13 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:66" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1200,40 +1208,40 @@
       <c r="U2" s="23"/>
       <c r="V2" s="15"/>
       <c r="W2" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
       <c r="Z2" s="23"/>
       <c r="AA2" s="16"/>
-      <c r="AB2" s="30" t="s">
+      <c r="AB2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
     </row>
     <row r="3" spans="2:66" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="39" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1260,12 +1268,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:66" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="24">
         <v>42797</v>
       </c>
@@ -1445,8 +1453,8 @@
       </c>
     </row>
     <row r="5" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
-        <v>28</v>
+      <c r="B5" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="27">
         <v>42797</v>
@@ -1466,8 +1474,8 @@
       <c r="AA5"/>
     </row>
     <row r="6" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
-        <v>29</v>
+      <c r="B6" s="31" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="27">
         <v>42800</v>
@@ -1487,7 +1495,7 @@
       <c r="AA6"/>
     </row>
     <row r="7" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="27">
@@ -1508,7 +1516,7 @@
       <c r="AA7"/>
     </row>
     <row r="8" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="31" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="27">
@@ -1529,7 +1537,7 @@
       <c r="AA8"/>
     </row>
     <row r="9" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="27">
@@ -1550,8 +1558,8 @@
       <c r="AA9"/>
     </row>
     <row r="10" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>18</v>
+      <c r="B10" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="27">
         <v>42806</v>
@@ -1566,13 +1574,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AA10"/>
     </row>
     <row r="11" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
-        <v>19</v>
+      <c r="B11" s="31" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="27">
         <v>42806</v>
@@ -1584,10 +1592,10 @@
         <v>42807</v>
       </c>
       <c r="F11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11"/>
     </row>
@@ -1602,7 +1610,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="27">
-        <v>42809</v>
+        <v>42808</v>
       </c>
       <c r="F12" s="5">
         <v>4</v>
@@ -1614,7 +1622,7 @@
     </row>
     <row r="13" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="27">
         <v>42810</v>
@@ -1635,7 +1643,7 @@
     </row>
     <row r="14" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="27">
         <v>42814</v>
@@ -1656,7 +1664,7 @@
     </row>
     <row r="15" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="27">
         <v>42815</v>
@@ -1677,7 +1685,7 @@
     </row>
     <row r="16" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="27">
         <v>42819</v>
@@ -1784,10 +1792,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,18 +1805,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish 70% auto form
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12150" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="13080" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
     <sheet name="Issue" sheetId="2" r:id="rId2"/>
+    <sheet name="Lesson" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Project Planner</t>
   </si>
@@ -263,6 +264,50 @@
   </si>
   <si>
     <t>delegate and invoke</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Structure</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Structure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>做得不够详细，导致实现的时候还要花时间想功能和逻辑。
+初期还是得尽量把所有事情都想明白。先不写</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>，在纸上把所有窗口
+画清楚。所有功能和逻辑想明白。</t>
+    </r>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -623,7 +668,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -745,6 +790,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1160,7 +1208,7 @@
   <dimension ref="B1:BN16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="26">
-        <v>42810</v>
+        <v>42811</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="19" t="s">
@@ -1625,7 +1673,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AA12"/>
     </row>
@@ -1804,7 +1852,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,4 +1889,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish AutoControl form and .ini read/write and temperature read/write
</commit_message>
<xml_diff>
--- a/Conduct_Auto_Temp_Control_Gantt.xlsx
+++ b/Conduct_Auto_Temp_Control_Gantt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="0" windowWidth="21600" windowHeight="9510"/>
+    <workbookView xWindow="14010" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -181,10 +181,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Auto Form</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>Chart Form</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -244,10 +240,6 @@
   </si>
   <si>
     <t>Step Control</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manual Form</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
@@ -308,6 +300,14 @@
       <t>，在纸上把所有窗口
 画清楚。所有功能和逻辑想明白。</t>
     </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual Form</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto Form</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -768,6 +768,9 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -790,9 +793,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1208,7 +1208,7 @@
   <dimension ref="B1:BN16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1232,13 +1232,13 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:66" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1265,40 +1265,40 @@
       <c r="U2" s="23"/>
       <c r="V2" s="15"/>
       <c r="W2" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X2" s="23"/>
       <c r="Y2" s="23"/>
       <c r="Z2" s="23"/>
       <c r="AA2" s="16"/>
-      <c r="AB2" s="33" t="s">
+      <c r="AB2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
     </row>
     <row r="3" spans="2:66" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="41" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1325,12 +1325,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:66" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="24">
         <v>42797</v>
       </c>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="5" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="27">
         <v>42797</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="6" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="27">
         <v>42800</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="9" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="27">
         <v>42805</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="10" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="27">
         <v>42806</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="11" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="27">
         <v>42806</v>
@@ -1657,8 +1657,8 @@
       <c r="AA11"/>
     </row>
     <row r="12" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
-        <v>16</v>
+      <c r="B12" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="C12" s="27">
         <v>42807</v>
@@ -1673,13 +1673,13 @@
         <v>3</v>
       </c>
       <c r="G12" s="6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AA12"/>
     </row>
     <row r="13" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
-        <v>28</v>
+      <c r="B13" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="C13" s="27">
         <v>42810</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="14" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="27">
         <v>42814</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="15" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="27">
         <v>42815</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="16" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="27">
         <v>42819</v>
@@ -1862,26 +1862,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1910,10 +1910,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>